<commit_message>
CPU Bound Benchmarking Done. SD Added.
</commit_message>
<xml_diff>
--- a/benchmark/results/3P_100M.xlsx
+++ b/benchmark/results/3P_100M.xlsx
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="3P_100M" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="612" uniqueCount="611">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="612">
   <si>
     <t>07/24/23 09:17:35.711304664</t>
   </si>
@@ -1852,14 +1852,19 @@
   </si>
   <si>
     <t>Value (in ms)</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+  <numFmts count="3">
+    <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+    <numFmt numFmtId="165" formatCode="0.000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -2338,8 +2343,10 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
@@ -2388,10 +2395,10 @@
   </cellStyles>
   <dxfs count="2">
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="164" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="166" formatCode="[$-F400]h:mm:ss\ AM/PM"/>
+      <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2407,12 +2414,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G1:I5" totalsRowShown="0">
-  <autoFilter ref="G1:I5"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="G1:I6" totalsRowShown="0">
+  <autoFilter ref="G1:I6"/>
   <tableColumns count="3">
     <tableColumn id="1" name="Aggregation"/>
     <tableColumn id="2" name="Value (in ns)"/>
-    <tableColumn id="3" name="Value (in ms)" dataDxfId="0">
+    <tableColumn id="3" name="Value (in ms)" dataDxfId="1">
       <calculatedColumnFormula>H2/(POWER(10,6))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -2424,7 +2431,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:E301" totalsRowShown="0">
   <autoFilter ref="A1:E301"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Producer Time Stamp" dataDxfId="1"/>
+    <tableColumn id="1" name="Producer Time Stamp" dataDxfId="0"/>
     <tableColumn id="2" name="Log Broker Time Stamp"/>
     <tableColumn id="3" name="Time Producer (in ns)">
       <calculatedColumnFormula>MID(A2,19,9)</calculatedColumnFormula>
@@ -2706,7 +2713,7 @@
   <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2864,7 +2871,7 @@
         <v>607</v>
       </c>
       <c r="H5">
-        <f>MAX(E2,E301)</f>
+        <f>MAX(E2:E301)</f>
         <v>1828837</v>
       </c>
       <c r="I5">
@@ -2890,6 +2897,17 @@
       <c r="E6">
         <f t="shared" si="3"/>
         <v>1383934</v>
+      </c>
+      <c r="G6" t="s">
+        <v>611</v>
+      </c>
+      <c r="H6" s="2">
+        <f>SQRT(_xlfn.VAR.S(E2:E301)/COUNT(E2:E301))</f>
+        <v>8473.8556115247375</v>
+      </c>
+      <c r="I6" s="3">
+        <f>H6/(POWER(10,6))</f>
+        <v>8.4738556115247377E-3</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>